<commit_message>
Bugfix: Materials without a hyphen were previously failing.
</commit_message>
<xml_diff>
--- a/testing/SPF Tests.xlsx
+++ b/testing/SPF Tests.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Side Projects\Successor Product Finder\Python-Successor-Finder\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8407C52-594D-4206-BE9A-F887F3E15E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9014EE60-1073-4604-A1F4-A195AC578EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expected Outputs" sheetId="1" r:id="rId1"/>
     <sheet name="v0.72b" sheetId="3" r:id="rId2"/>
+    <sheet name="v0.8b" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="91">
   <si>
     <t>Input Material</t>
   </si>
@@ -233,13 +234,79 @@
   </si>
   <si>
     <t>Active Product</t>
+  </si>
+  <si>
+    <t>5MMDDR.4096-04</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>5AC901.HS00-01</t>
+  </si>
+  <si>
+    <t>This successor is intended for the TS-17 (QM170/HM170) system units.</t>
+  </si>
+  <si>
+    <t>X20CP1585</t>
+  </si>
+  <si>
+    <t>No direct successor found. Look into the appropriate interfaces for the system you are upgrading to.</t>
+  </si>
+  <si>
+    <t>No direct successor. The B&amp;R 2005 system is too outdated to provide a comparable successor. Projects should be changed over to X20.</t>
+  </si>
+  <si>
+    <t>No direct successor. The B&amp;R 2003 system is too outdated to provide a comparable successor. Projects should be changed over to X20.</t>
+  </si>
+  <si>
+    <t>8AC110.60-3</t>
+  </si>
+  <si>
+    <t>No direct successor. Look at X20 PLCs for the appropriate successor.</t>
+  </si>
+  <si>
+    <t>The input material is custom, please speak with the machine manufacturer for upgrade options.</t>
+  </si>
+  <si>
+    <t>No direct successor. The appropriate successor will be one of the P86 8I0IFENC.xxx-1 encoder interfaces.</t>
+  </si>
+  <si>
+    <t>No direct successor. Transition to the ACOPOS P3 or ACOPOSmulti series.</t>
+  </si>
+  <si>
+    <t>The input material is valid. However, there unfortunately is no successor product.</t>
+  </si>
+  <si>
+    <t>No direct successor. The listed successor is the Power Panel 65 series. However, that series is also obsolete. Transition to a Power Panel C-Series device or a Power Panel T30 with a X20CP Compact-S depending on demands of the application. See sales notice 38/2021.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfortunately, a successor product for the entered material number is not available. The entered material is either not obsolete, there are mistakes in your input or this program is missing this material. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The material number entered was for a Windows operating system. It's successor operating system is dependent on the compatibility of the target PC.Unfortunately, a successor product for the entered material number is not available. The entered material is either not obsolete, there are mistakes in your input or this program is missing this material. </t>
+  </si>
+  <si>
+    <t>No direct successor. Transition to the appropriate TS17 (5PC900.TS17-xx) CPU board depending on performance needed.</t>
+  </si>
+  <si>
+    <t>No direct successor. Go to Y:\Application\Support Team\KnowledgeBase\Hardware\Motors\MotorConversions\MSA Motor Lookup v01.1.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8I74T400075.010-1: The material numbered entered is the base module for the ACOPOS inverter and is still in production. Please enter the 8I74T4xxxxx.01P-1 material number.Unfortunately, a successor product for the entered material number is not available. The entered material is either not obsolete, there are mistakes in your input or this program is missing this material. </t>
+  </si>
+  <si>
+    <t>Software changes are not necessary if the panel is connected to an APC via SDL.</t>
+  </si>
+  <si>
+    <t>No direct successor. Transition to a Power Panel C-Series device or a Power Panel T30 with a X20CP Compact-S depending on demands of the application. See sales notice 38/2021.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,8 +337,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="MS Shell Dlg 2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,8 +356,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -302,12 +380,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -315,16 +408,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -358,6 +481,19 @@
     <tableColumn id="2" xr3:uid="{C306F41D-1BDE-48D6-990E-B47BD318588E}" name="Successor Output"/>
     <tableColumn id="3" xr3:uid="{E857FA80-6979-4DD6-BF3F-DFC0DA92274B}" name="SW Changes"/>
     <tableColumn id="4" xr3:uid="{AD245590-506F-480A-97F3-ED7761F90FB9}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21E50D56-CA3E-4F63-BC87-B16263BD5423}" name="Table462" displayName="Table462" ref="A1:D40" totalsRowShown="0">
+  <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C52E1E9D-D826-4F8F-875A-0A4CCFF198B5}" name="Input Material"/>
+    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,10 +764,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +858,7 @@
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -750,7 +886,7 @@
       <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -764,12 +900,12 @@
       <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
@@ -783,16 +919,16 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="4"/>
+      <c r="B11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -804,7 +940,7 @@
       <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -818,7 +954,7 @@
       <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -832,24 +968,26 @@
       <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="B15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
@@ -858,7 +996,7 @@
       <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -886,7 +1024,7 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -900,7 +1038,7 @@
       <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -912,7 +1050,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -941,22 +1079,22 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="4"/>
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C24" t="s">
@@ -964,16 +1102,18 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="4"/>
+      <c r="B25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -987,28 +1127,30 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="4"/>
+      <c r="B27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="4"/>
+      <c r="B28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1020,18 +1162,23 @@
       <c r="C29" t="s">
         <v>47</v>
       </c>
+      <c r="D29" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="4"/>
+      <c r="B30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1043,7 +1190,7 @@
       <c r="C31" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1051,13 +1198,15 @@
       <c r="A32" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="B32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1074,16 +1223,18 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="4"/>
+      <c r="B34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1108,22 +1259,24 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="4"/>
+      <c r="B37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C38" t="s">
@@ -1131,16 +1284,18 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="4"/>
+      <c r="B39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1166,9 +1321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C80A962-FF4F-4079-A2D9-ADFB05B6F941}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D22" sqref="D22:D39"/>
+      <selection pane="topRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,10 +1348,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1270,7 +1425,7 @@
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1298,7 +1453,7 @@
       <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1312,7 +1467,7 @@
       <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1354,7 +1509,7 @@
       <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1368,7 +1523,7 @@
       <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1382,7 +1537,7 @@
       <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1410,7 +1565,7 @@
       <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1438,7 +1593,7 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1452,7 +1607,7 @@
       <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1463,8 +1618,8 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
-        <v>46</v>
+      <c r="C20" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,7 +1760,7 @@
       <c r="C31" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1738,4 +1893,534 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D085407D-DDC4-4B61-A41D-FFE8402C48A9}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added PROVIT and PC Configuration Support
</commit_message>
<xml_diff>
--- a/testing/SPF Tests.xlsx
+++ b/testing/SPF Tests.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Side Projects\Successor Product Finder\Python-Successor-Finder\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAB4E56-1041-45B2-9DE2-9C98BD9EBD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98B21B1-E54F-496F-B945-70B340F313D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expected Outputs" sheetId="1" r:id="rId1"/>
     <sheet name="v0.72b" sheetId="3" r:id="rId2"/>
     <sheet name="v0.8b" sheetId="4" r:id="rId3"/>
     <sheet name="v0.81b" sheetId="5" r:id="rId4"/>
+    <sheet name="v0.82b" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="112">
   <si>
     <t>Input Material</t>
   </si>
@@ -325,6 +326,45 @@
   </si>
   <si>
     <t>No direct successor. The B&amp;R 2003 system is too outdated to provide a comparable successor. Projects should be changed over to X20</t>
+  </si>
+  <si>
+    <t>8I64S200110.000-1</t>
+  </si>
+  <si>
+    <t>5W5C000002A107-001</t>
+  </si>
+  <si>
+    <t>5C3002.0</t>
+  </si>
+  <si>
+    <t>5TCZC4AC0000M0-001  </t>
+  </si>
+  <si>
+    <t>5ZBB0525007100-000</t>
+  </si>
+  <si>
+    <t>5WEA0000012407-000</t>
+  </si>
+  <si>
+    <t>5Q5C0000I1130F-000</t>
+  </si>
+  <si>
+    <t>5Y0SE060000000-000</t>
+  </si>
+  <si>
+    <t>5ACEW011010000-000</t>
+  </si>
+  <si>
+    <t>5Z6B0SB42500R0-001</t>
+  </si>
+  <si>
+    <t>5R3A200000000F-001</t>
+  </si>
+  <si>
+    <t>5FE3100000A0Q0-000</t>
+  </si>
+  <si>
+    <t>5S4EDD001000V0-000</t>
   </si>
 </sst>
 </file>
@@ -425,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -445,12 +485,53 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -559,22 +640,35 @@
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C52E1E9D-D826-4F8F-875A-0A4CCFF198B5}" name="Input Material"/>
-    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5173076C-01CF-40A1-AF29-B9F05408AED6}" name="Table46234" displayName="Table46234" ref="A1:D53" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D53" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0F8ED474-F344-4023-8D80-EE36506904CF}" name="Input Material" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{06FACCA0-1A0F-4361-9D94-DD0154716F72}" name="Successor Output" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C1747EA0-BE16-4D3F-AC43-33907F6A45EC}" name="SW Changes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{CE012C2D-E713-4D55-BC75-CD9D689B0768}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,15 +945,15 @@
       <selection pane="topRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="248.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -887,7 +981,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -901,7 +995,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -915,7 +1009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -929,7 +1023,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -943,7 +1037,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -957,7 +1051,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -971,7 +1065,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -985,7 +1079,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -999,7 +1093,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1011,7 +1105,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1025,7 +1119,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1039,7 +1133,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1053,7 +1147,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1161,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1081,7 +1175,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1095,7 +1189,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1109,7 +1203,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1123,7 +1217,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1134,7 +1228,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1145,7 +1239,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1159,7 +1253,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1171,7 +1265,7 @@
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1276,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
@@ -1196,7 +1290,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1207,7 +1301,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
@@ -1221,7 +1315,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
@@ -1233,7 +1327,7 @@
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1247,7 +1341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
@@ -1261,7 +1355,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1275,7 +1369,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>32</v>
       </c>
@@ -1289,7 +1383,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1303,7 +1397,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1317,7 +1411,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1328,7 +1422,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1339,7 +1433,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1353,7 +1447,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1364,7 +1458,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -1378,7 +1472,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1410,16 +1504,16 @@
       <selection pane="topRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="248.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1531,7 @@
       </c>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1457,7 +1551,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +1565,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1485,7 +1579,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1499,7 +1593,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1513,7 +1607,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1527,7 +1621,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1541,7 +1635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1555,7 +1649,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1663,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1583,7 +1677,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1597,7 +1691,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +1705,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1625,7 +1719,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1639,7 +1733,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1653,7 +1747,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1667,7 +1761,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1681,7 +1775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1695,7 +1789,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1706,7 +1800,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1717,7 +1811,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1731,7 +1825,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1745,7 +1839,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1756,7 +1850,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1770,7 +1864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1781,7 +1875,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1795,7 +1889,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -1809,7 +1903,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1820,7 +1914,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1834,7 +1928,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1848,7 +1942,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1862,7 +1956,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1876,7 +1970,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1890,7 +1984,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1901,7 +1995,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1912,7 +2006,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1926,7 +2020,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1937,7 +2031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1951,7 +2045,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1988,16 +2082,16 @@
       <selection pane="topRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="248.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2109,7 @@
       </c>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2035,7 +2129,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2049,7 +2143,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2063,7 +2157,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2077,7 +2171,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2091,7 +2185,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2105,7 +2199,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2119,7 +2213,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2133,7 +2227,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -2147,7 +2241,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2159,7 +2253,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2173,7 +2267,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2187,7 +2281,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2201,7 +2295,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -2215,7 +2309,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -2229,7 +2323,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2243,7 +2337,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -2251,7 +2345,7 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
@@ -2259,7 +2353,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2271,7 +2365,7 @@
       </c>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2283,7 +2377,7 @@
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2297,7 +2391,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2309,7 +2403,7 @@
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
@@ -2317,7 +2411,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
@@ -2325,7 +2419,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2337,7 +2431,7 @@
       </c>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>27</v>
       </c>
@@ -2345,7 +2439,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -2357,7 +2451,7 @@
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2369,7 +2463,7 @@
       </c>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>30</v>
       </c>
@@ -2377,7 +2471,7 @@
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2391,7 +2485,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>32</v>
       </c>
@@ -2399,7 +2493,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -2413,7 +2507,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2427,7 +2521,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2439,7 +2533,7 @@
       </c>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2451,7 +2545,7 @@
       </c>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -2465,7 +2559,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -2477,7 +2571,7 @@
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>41</v>
       </c>
@@ -2485,7 +2579,7 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2513,21 +2607,603 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD6CAA4E-9A4A-48D5-ABD5-6781005958F2}">
   <dimension ref="A1:G40"/>
   <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FFE3A1-4275-4B18-B910-53ACB0B76F80}">
+  <dimension ref="A1:G53"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="248.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2545,19 +3221,13 @@
       </c>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
       <c r="F2" s="3" t="s">
         <v>44</v>
       </c>
@@ -2565,519 +3235,413 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Corrected Resolver Code For 8LSA/8LSC
</commit_message>
<xml_diff>
--- a/testing/SPF Tests.xlsx
+++ b/testing/SPF Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Side Projects\Successor Product Finder\Python-Successor-Finder\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003C4546-87B9-43A0-AD04-7EAB8B2C09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12195C4-AFCC-4C0F-A229-3133FCC036BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expected Outputs" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="v0.8b" sheetId="4" r:id="rId3"/>
     <sheet name="v0.81b" sheetId="5" r:id="rId4"/>
     <sheet name="v0.82b" sheetId="6" r:id="rId5"/>
+    <sheet name="v0.83b" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="266">
   <si>
     <t>Input Material</t>
   </si>
@@ -806,6 +807,27 @@
   </si>
   <si>
     <t xml:space="preserve">5S4EDD001000V0-000: The material number entered was for a configuration. Speak with a sales representative to determine the best upgrade for the application. </t>
+  </si>
+  <si>
+    <t>8LSC5C.R0030D305-0</t>
+  </si>
+  <si>
+    <t>8LSA46.R0022D100-0 -&gt; 8LSA46.R2022D100-3</t>
+  </si>
+  <si>
+    <t>8LSC5C.R0030D305-0 -&gt; 8LSC5C.R2030D305-3</t>
+  </si>
+  <si>
+    <t>8LSC5C.R0030D305-0: yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5SWWI7.1540-ENG: The material number entered was for a Windows operating system. It's successor operating system is dependent on the compatibility of the successor target PC. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8LSA46.R0022D100-0: Confirm this is the correct successor with the Support. Send an email to support.us@br-automation.com. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8LSC5C.R0030D305-0: Confirm this is the correct successor with the Support. Send an email to support.us@br-automation.com. </t>
   </si>
 </sst>
 </file>
@@ -849,7 +871,7 @@
       <name val="MS Shell Dlg 2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -865,6 +887,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -906,7 +934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -927,12 +955,53 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1081,35 +1150,48 @@
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C52E1E9D-D826-4F8F-875A-0A4CCFF198B5}" name="Input Material"/>
-    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5173076C-01CF-40A1-AF29-B9F05408AED6}" name="Table46234" displayName="Table46234" ref="A1:D54" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5173076C-01CF-40A1-AF29-B9F05408AED6}" name="Table46234" displayName="Table46234" ref="A1:D54" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:D54" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0F8ED474-F344-4023-8D80-EE36506904CF}" name="Input Material" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{06FACCA0-1A0F-4361-9D94-DD0154716F72}" name="Successor Output" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C1747EA0-BE16-4D3F-AC43-33907F6A45EC}" name="SW Changes" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{CE012C2D-E713-4D55-BC75-CD9D689B0768}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0F8ED474-F344-4023-8D80-EE36506904CF}" name="Input Material" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{06FACCA0-1A0F-4361-9D94-DD0154716F72}" name="Successor Output" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C1747EA0-BE16-4D3F-AC43-33907F6A45EC}" name="SW Changes" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{CE012C2D-E713-4D55-BC75-CD9D689B0768}" name="Notes" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{171B1F0B-8AD4-4805-B607-F75AC71ABC67}" name="Table462347" displayName="Table462347" ref="A1:D55" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D55" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5B4C4599-C37F-423B-B36A-E3E0509870EB}" name="Input Material" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4009E4CB-EF82-49EA-8B4D-2E10B6297D3D}" name="Successor Output" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{32CB6C97-357F-4606-803F-28493B4B11A6}" name="SW Changes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{02E0E45A-EF85-4E8B-A4C0-2F0EF20C43E2}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1378,12 +1460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="D7" sqref="D7"/>
+      <selection pane="topRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3630,9 +3715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FFE3A1-4275-4B18-B910-53ACB0B76F80}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C36" sqref="C36"/>
+      <selection pane="topRight" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4394,4 +4479,783 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BBCF00-319F-4066-AC9A-00D67EF77ADB}">
+  <dimension ref="A1:G55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Slight correction for P74 inverters
</commit_message>
<xml_diff>
--- a/testing/SPF Tests.xlsx
+++ b/testing/SPF Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Side Projects\Successor Product Finder\Python-Successor-Finder\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12195C4-AFCC-4C0F-A229-3133FCC036BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548A76BE-98CE-43C3-BC49-A903F75F14FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expected Outputs" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="v0.81b" sheetId="5" r:id="rId4"/>
     <sheet name="v0.82b" sheetId="6" r:id="rId5"/>
     <sheet name="v0.83b" sheetId="7" r:id="rId6"/>
+    <sheet name="v0.84" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="294">
   <si>
     <t>Input Material</t>
   </si>
@@ -828,6 +829,90 @@
   </si>
   <si>
     <t xml:space="preserve">8LSC5C.R0030D305-0: Confirm this is the correct successor with the Support. Send an email to support.us@br-automation.com. </t>
+  </si>
+  <si>
+    <t>5AP820.1505-00</t>
+  </si>
+  <si>
+    <t>5AP820.1505-K02</t>
+  </si>
+  <si>
+    <t>5WB6W0310AB060-001</t>
+  </si>
+  <si>
+    <t>5AP820.1505-00 -&gt; 5AP5120.1505-000 + 5DLSDL.1001-00</t>
+  </si>
+  <si>
+    <t>5AP820.1505-K02 -&gt; N/A</t>
+  </si>
+  <si>
+    <t>5WB6W0310AB060-001 -&gt; N/A</t>
+  </si>
+  <si>
+    <t>5AP820.1505-00: yes</t>
+  </si>
+  <si>
+    <t>5AP820.1505-K02: yes</t>
+  </si>
+  <si>
+    <t>5WB6W0310AB060-001: N/A</t>
+  </si>
+  <si>
+    <t>8V1180.00-2: No specific successor listed. Transition to the ACOPOS P3 or ACOPOSmulti series.</t>
+  </si>
+  <si>
+    <t>4PP045.0571-042: No specific successor listed. The listed successor is the Power Panel 65 series. However, that series is also obsolete. Transition to a Power Panel C-Series device or a Power Panel T30 with a X20CP Compact-S depending on demands of the application. See sales notice 38/2021.</t>
+  </si>
+  <si>
+    <t>4PP045.IF23-1: No specific successor listed. Look into the appropriate interfaces for the system you are upgrading to. Speak with a sales representative to determine the best upgrade for the application.</t>
+  </si>
+  <si>
+    <t>5AC901.FF01-00: No specific successor listed. The appropriate successor is dependent on the successor PC. Speak with a sales representative to determine the best upgrade for the application.</t>
+  </si>
+  <si>
+    <t>5PC900.TS77-05: No specific successor listed. Transition to the appropriate TS17 (5PC900.TS17-xx) CPU board depending on performance needed.</t>
+  </si>
+  <si>
+    <t>5AC901.BX01-00: No specific successor listed. The appropriate successor is dependent on the successor PC. Speak with a sales representative to determine the best upgrade for the application.</t>
+  </si>
+  <si>
+    <t>5AC901.HS00-00: No specific successor listed. The appropriate heatsink will be associated with the successor PC. Speak with a sales representative to determine the best upgrade for the application.</t>
+  </si>
+  <si>
+    <t>5AC901.FA01-00: No specific successor listed. The appropriate fan will be associated with the successor PC. Speak with a sales representative to determine the best upgrade for the application.</t>
+  </si>
+  <si>
+    <t>8MSA4X.R0-30: No specific successor listed. Go to Y:\Application\Support Team\KnowledgeBase\Hardware\Motors\MotorConversions\MSA Motor Lookup v01.1.xlsx</t>
+  </si>
+  <si>
+    <t>X20CP1382: No specific successor listed. Look at X20 PLCs for the appropriate successor. Speak with a sales representative to determine the best fit for the application.</t>
+  </si>
+  <si>
+    <t>4PP065.0571-P74: No specific successor listed. Transition to a Power Panel C-Series device or a Power Panel T30 with a X20CP Compact-S depending on demands of the application. See sales notice 38/2021.</t>
+  </si>
+  <si>
+    <t>5PP5IF.FPLM-00: No specific successor listed. Look into the appropriate interfaces for the system you are upgrading to. Speak with a sales representative to determine the best upgrade for the application.</t>
+  </si>
+  <si>
+    <t>8I0AC123.301-1: No specific successor listed. The appropriate successor will be one of the P86 8I0IFENC.xxx-1 encoder interfaces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5AP820.1505-00: Software changes are not necessary if the panel is connected to an APC via SDL. </t>
+  </si>
+  <si>
+    <t>5AP820.1505-K02: The input material is custom, please speak with the machine manufacturer for upgrade options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5WB6W0310AB060-001: The material number entered was for a configuration. Speak with a sales representative to determine the best upgrade for the application. </t>
+  </si>
+  <si>
+    <t>Please ensure successor(s) is (are) not obsolete too.</t>
+  </si>
+  <si>
+    <t>8I74T400075.010-1 -&gt; 8I74S200075.0P-000 + 8I76S200075.00-000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8I74T400075.010-1: The base device and communication card 8I74S200075.0P-000 + 8I76S200075.00-000 must be ordered together. </t>
   </si>
 </sst>
 </file>
@@ -954,14 +1039,54 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1150,48 +1275,61 @@
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C52E1E9D-D826-4F8F-875A-0A4CCFF198B5}" name="Input Material"/>
-    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5173076C-01CF-40A1-AF29-B9F05408AED6}" name="Table46234" displayName="Table46234" ref="A1:D54" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5173076C-01CF-40A1-AF29-B9F05408AED6}" name="Table46234" displayName="Table46234" ref="A1:D54" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:D54" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0F8ED474-F344-4023-8D80-EE36506904CF}" name="Input Material" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{06FACCA0-1A0F-4361-9D94-DD0154716F72}" name="Successor Output" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{C1747EA0-BE16-4D3F-AC43-33907F6A45EC}" name="SW Changes" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{CE012C2D-E713-4D55-BC75-CD9D689B0768}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{0F8ED474-F344-4023-8D80-EE36506904CF}" name="Input Material" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{06FACCA0-1A0F-4361-9D94-DD0154716F72}" name="Successor Output" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{C1747EA0-BE16-4D3F-AC43-33907F6A45EC}" name="SW Changes" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{CE012C2D-E713-4D55-BC75-CD9D689B0768}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{171B1F0B-8AD4-4805-B607-F75AC71ABC67}" name="Table462347" displayName="Table462347" ref="A1:D55" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{171B1F0B-8AD4-4805-B607-F75AC71ABC67}" name="Table462347" displayName="Table462347" ref="A1:D55" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:D55" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5B4C4599-C37F-423B-B36A-E3E0509870EB}" name="Input Material" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4009E4CB-EF82-49EA-8B4D-2E10B6297D3D}" name="Successor Output" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{32CB6C97-357F-4606-803F-28493B4B11A6}" name="SW Changes" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{02E0E45A-EF85-4E8B-A4C0-2F0EF20C43E2}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5B4C4599-C37F-423B-B36A-E3E0509870EB}" name="Input Material" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{4009E4CB-EF82-49EA-8B4D-2E10B6297D3D}" name="Successor Output" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{32CB6C97-357F-4606-803F-28493B4B11A6}" name="SW Changes" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{02E0E45A-EF85-4E8B-A4C0-2F0EF20C43E2}" name="Notes" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C8A56E0E-9BB3-48BC-9FB6-05AE9047B426}" name="Table4623478" displayName="Table4623478" ref="A1:D58" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D58" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{24E5E3F4-6598-4525-8ED3-F71DFFCEB6A0}" name="Input Material" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{F1B6E2FB-D441-42D6-B61F-315C240DF788}" name="Successor Output" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{404954E4-0555-4BA1-9929-C28C7647DDA3}" name="SW Changes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{AA55FC73-C3D9-4417-81EB-CA854C43A185}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2052,10 +2190,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2630,10 +2768,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3160,10 +3298,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3742,10 +3880,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -4485,9 +4623,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BBCF00-319F-4066-AC9A-00D67EF77ADB}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4512,8 +4650,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -4610,7 +4748,7 @@
       <c r="C8" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>222</v>
       </c>
     </row>
@@ -4624,7 +4762,7 @@
       <c r="C9" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>223</v>
       </c>
     </row>
@@ -4664,7 +4802,7 @@
       <c r="C12" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4692,7 +4830,7 @@
       <c r="C14" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>227</v>
       </c>
     </row>
@@ -4748,7 +4886,7 @@
       <c r="C18" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4762,7 +4900,7 @@
       <c r="C19" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4796,7 +4934,7 @@
       <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>132</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -4920,7 +5058,7 @@
       <c r="C31" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
         <v>238</v>
       </c>
     </row>
@@ -5247,6 +5385,829 @@
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51A7032-F6A8-4452-A7EC-EAF1644F4767}">
+  <dimension ref="A1:G58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D56" sqref="D56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>268</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>291</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
4B1300.02-510 Added To Testing Spreadsheet
</commit_message>
<xml_diff>
--- a/testing/SPF Tests.xlsx
+++ b/testing/SPF Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Side Projects\Successor Product Finder\Python-Successor-Finder\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627B0385-C523-4CEA-AFE3-8FE33B999E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4443C1-56CC-4689-8BC5-1F47C06122F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expected Outputs" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="v0.82b" sheetId="6" r:id="rId5"/>
     <sheet name="v0.83b" sheetId="7" r:id="rId6"/>
     <sheet name="v0.84" sheetId="9" r:id="rId7"/>
+    <sheet name="v0.85" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="295">
   <si>
     <t>Input Material</t>
   </si>
@@ -913,6 +914,9 @@
   </si>
   <si>
     <t xml:space="preserve">8I74T400075.010-1: The base device and communication card 8I74S200075.0P-000 + 8I76S200075.00-000 must be ordered together. </t>
+  </si>
+  <si>
+    <t>4B1300.02-510</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1050,47 @@
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1275,61 +1319,74 @@
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C52E1E9D-D826-4F8F-875A-0A4CCFF198B5}" name="Input Material"/>
-    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{D6F160D5-877D-485D-AA5E-5F45D6DC2994}" name="Successor Output" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{DCF14BF5-F7F2-4E2A-B350-FEDD0FA1875E}" name="SW Changes" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{AD5F1D88-ACAE-467B-BC19-547388B251B5}" name="Notes" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E795633-7505-4D4A-A1BC-A741ED5C1777}" name="Table4623" displayName="Table4623" ref="A1:D40" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="A1:D40" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{4071701F-6725-43C3-987E-C73B834A8A73}" name="Input Material" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{6F68F9F6-8589-47D7-AEF9-FFAE6C00A7C5}" name="Successor Output" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{90C1C7DE-88A5-4B22-9B18-8C9C7C00E49D}" name="SW Changes" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{AF6C7701-9F31-4A7A-99D7-F3097611F2C9}" name="Notes" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5173076C-01CF-40A1-AF29-B9F05408AED6}" name="Table46234" displayName="Table46234" ref="A1:D54" totalsRowShown="0" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5173076C-01CF-40A1-AF29-B9F05408AED6}" name="Table46234" displayName="Table46234" ref="A1:D54" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="A1:D54" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0F8ED474-F344-4023-8D80-EE36506904CF}" name="Input Material" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{06FACCA0-1A0F-4361-9D94-DD0154716F72}" name="Successor Output" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{C1747EA0-BE16-4D3F-AC43-33907F6A45EC}" name="SW Changes" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{CE012C2D-E713-4D55-BC75-CD9D689B0768}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{0F8ED474-F344-4023-8D80-EE36506904CF}" name="Input Material" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{06FACCA0-1A0F-4361-9D94-DD0154716F72}" name="Successor Output" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{C1747EA0-BE16-4D3F-AC43-33907F6A45EC}" name="SW Changes" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{CE012C2D-E713-4D55-BC75-CD9D689B0768}" name="Notes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{171B1F0B-8AD4-4805-B607-F75AC71ABC67}" name="Table462347" displayName="Table462347" ref="A1:D55" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{171B1F0B-8AD4-4805-B607-F75AC71ABC67}" name="Table462347" displayName="Table462347" ref="A1:D55" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:D55" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5B4C4599-C37F-423B-B36A-E3E0509870EB}" name="Input Material" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{4009E4CB-EF82-49EA-8B4D-2E10B6297D3D}" name="Successor Output" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{32CB6C97-357F-4606-803F-28493B4B11A6}" name="SW Changes" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{02E0E45A-EF85-4E8B-A4C0-2F0EF20C43E2}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{5B4C4599-C37F-423B-B36A-E3E0509870EB}" name="Input Material" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{4009E4CB-EF82-49EA-8B4D-2E10B6297D3D}" name="Successor Output" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{32CB6C97-357F-4606-803F-28493B4B11A6}" name="SW Changes" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{02E0E45A-EF85-4E8B-A4C0-2F0EF20C43E2}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C8A56E0E-9BB3-48BC-9FB6-05AE9047B426}" name="Table4623478" displayName="Table4623478" ref="A1:D58" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D58" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C8A56E0E-9BB3-48BC-9FB6-05AE9047B426}" name="Table4623478" displayName="Table4623478" ref="A1:D59" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D59" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{24E5E3F4-6598-4525-8ED3-F71DFFCEB6A0}" name="Input Material" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{F1B6E2FB-D441-42D6-B61F-315C240DF788}" name="Successor Output" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{404954E4-0555-4BA1-9929-C28C7647DDA3}" name="SW Changes" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{AA55FC73-C3D9-4417-81EB-CA854C43A185}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{24E5E3F4-6598-4525-8ED3-F71DFFCEB6A0}" name="Input Material" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F1B6E2FB-D441-42D6-B61F-315C240DF788}" name="Successor Output" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{404954E4-0555-4BA1-9929-C28C7647DDA3}" name="SW Changes" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{AA55FC73-C3D9-4417-81EB-CA854C43A185}" name="Notes" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E542D401-AB79-423D-A6E4-FB2C7ED5BDB4}" name="Table46234789" displayName="Table46234789" ref="A1:D59" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D59" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0B417A11-B69D-401D-A473-886E33816374}" name="Input Material" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{8DE7CB05-6377-4ABC-B741-312F0785E7FB}" name="Successor Output" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4671D6A9-4733-4BE3-B687-16C4F5C50AB4}" name="SW Changes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DBD28084-575B-48FA-872C-1BF0B9D476E8}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5400,11 +5457,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51A7032-F6A8-4452-A7EC-EAF1644F4767}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:A33"/>
+      <selection pane="topRight" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6205,7 +6262,524 @@
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE714DD0-B449-4CA1-B4CF-4E20A651A778}">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D49" sqref="D49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="248.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>268</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5" t="s">
         <v>291</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 9A0100.11 to Testing Spreadsheet
</commit_message>
<xml_diff>
--- a/testing/SPF Tests.xlsx
+++ b/testing/SPF Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Side Projects\Successor Product Finder\Python-Successor-Finder\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4443C1-56CC-4689-8BC5-1F47C06122F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9FAAF3-625F-406A-8322-051A4F8F844B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="296">
   <si>
     <t>Input Material</t>
   </si>
@@ -917,6 +917,9 @@
   </si>
   <si>
     <t>4B1300.02-510</t>
+  </si>
+  <si>
+    <t>9A0100.11</t>
   </si>
 </sst>
 </file>
@@ -1380,8 +1383,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E542D401-AB79-423D-A6E4-FB2C7ED5BDB4}" name="Table46234789" displayName="Table46234789" ref="A1:D59" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D59" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E542D401-AB79-423D-A6E4-FB2C7ED5BDB4}" name="Table46234789" displayName="Table46234789" ref="A1:D60" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D60" xr:uid="{CC11B020-A102-443F-9499-3057248983DE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0B417A11-B69D-401D-A473-886E33816374}" name="Input Material" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{8DE7CB05-6377-4ABC-B741-312F0785E7FB}" name="Successor Output" dataDxfId="2"/>
@@ -6286,11 +6289,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE714DD0-B449-4CA1-B4CF-4E20A651A778}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D49" sqref="D49"/>
+      <selection pane="topRight" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6776,10 +6779,18 @@
       <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+      <c r="A59" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5" t="s">
         <v>291</v>
       </c>
     </row>

</xml_diff>